<commit_message>
C Array vs Struct
</commit_message>
<xml_diff>
--- a/MatMul_bench.xlsx
+++ b/MatMul_bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eakis\source\repos\EvgeniyKishov\matmul_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C56EC-6524-4C70-96BD-B0A6D18D447D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1EBF8-8343-4121-BC28-8C4C03890365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>C# Parallel</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>C Parallel</t>
+  </si>
+  <si>
+    <t>C array</t>
+  </si>
+  <si>
+    <t>C array parallel</t>
   </si>
 </sst>
 </file>
@@ -1432,16 +1438,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1732,18 +1738,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2</v>
       </c>
@@ -1759,8 +1766,14 @@
       <c r="E1">
         <v>0</v>
       </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1776,8 +1789,14 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>500</v>
       </c>
@@ -1793,8 +1812,14 @@
       <c r="E3">
         <v>67</v>
       </c>
+      <c r="F3">
+        <v>162</v>
+      </c>
+      <c r="G3">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -1810,8 +1835,14 @@
       <c r="E4">
         <v>681</v>
       </c>
+      <c r="F4">
+        <v>2077</v>
+      </c>
+      <c r="G4">
+        <v>677</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -1827,8 +1858,14 @@
       <c r="E5">
         <v>6771</v>
       </c>
+      <c r="F5">
+        <v>39660</v>
+      </c>
+      <c r="G5">
+        <v>6075</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1843,6 +1880,12 @@
       </c>
       <c r="E6" t="s">
         <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>